<commit_message>
done synchronize with google sheets
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t xml:space="preserve">Меню</t>
+    <t xml:space="preserve">меню3</t>
   </si>
   <si>
     <t xml:space="preserve">Основное меню</t>
@@ -271,16 +271,16 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="77.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>